<commit_message>
Change index column of user and post table
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_QuangVo.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_QuangVo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="0" windowWidth="16340" windowHeight="14080" tabRatio="818" activeTab="3"/>
+    <workbookView xWindow="4000" yWindow="240" windowWidth="16340" windowHeight="14080" tabRatio="818" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="214">
   <si>
     <t>No</t>
   </si>
@@ -697,9 +697,6 @@
   </si>
   <si>
     <t>image</t>
-  </si>
-  <si>
-    <t>LONGBLOB</t>
   </si>
   <si>
     <t>TIMESTAMP</t>
@@ -965,7 +962,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="87">
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -1804,28 +1801,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -2141,6 +2116,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="458">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3515,7 +3570,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3876,15 +3931,6 @@
     <xf numFmtId="49" fontId="28" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3954,40 +4000,37 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4002,34 +4045,34 @@
     <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4055,6 +4098,21 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4180,40 +4238,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="2" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4222,26 +4277,56 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="86" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="458">
@@ -5948,29 +6033,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="194"/>
-      <c r="P13" s="194"/>
-      <c r="Q13" s="194"/>
-      <c r="R13" s="194"/>
-      <c r="S13" s="194"/>
-      <c r="T13" s="194"/>
-      <c r="U13" s="194"/>
-      <c r="V13" s="194"/>
-      <c r="W13" s="194"/>
-      <c r="X13" s="194"/>
-      <c r="Y13" s="194"/>
-      <c r="Z13" s="194"/>
-      <c r="AA13" s="194"/>
-      <c r="AB13" s="194"/>
-      <c r="AC13" s="194"/>
-      <c r="AD13" s="194"/>
-      <c r="AE13" s="194"/>
-      <c r="AF13" s="194"/>
-      <c r="AG13" s="194"/>
-      <c r="AH13" s="194"/>
-      <c r="AI13" s="194"/>
-      <c r="AJ13" s="194"/>
-      <c r="AK13" s="194"/>
+      <c r="O13" s="195"/>
+      <c r="P13" s="195"/>
+      <c r="Q13" s="195"/>
+      <c r="R13" s="195"/>
+      <c r="S13" s="195"/>
+      <c r="T13" s="195"/>
+      <c r="U13" s="195"/>
+      <c r="V13" s="195"/>
+      <c r="W13" s="195"/>
+      <c r="X13" s="195"/>
+      <c r="Y13" s="195"/>
+      <c r="Z13" s="195"/>
+      <c r="AA13" s="195"/>
+      <c r="AB13" s="195"/>
+      <c r="AC13" s="195"/>
+      <c r="AD13" s="195"/>
+      <c r="AE13" s="195"/>
+      <c r="AF13" s="195"/>
+      <c r="AG13" s="195"/>
+      <c r="AH13" s="195"/>
+      <c r="AI13" s="195"/>
+      <c r="AJ13" s="195"/>
+      <c r="AK13" s="195"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -6002,29 +6087,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="194"/>
-      <c r="P14" s="194"/>
-      <c r="Q14" s="194"/>
-      <c r="R14" s="194"/>
-      <c r="S14" s="194"/>
-      <c r="T14" s="194"/>
-      <c r="U14" s="194"/>
-      <c r="V14" s="194"/>
-      <c r="W14" s="194"/>
-      <c r="X14" s="194"/>
-      <c r="Y14" s="194"/>
-      <c r="Z14" s="194"/>
-      <c r="AA14" s="194"/>
-      <c r="AB14" s="194"/>
-      <c r="AC14" s="194"/>
-      <c r="AD14" s="194"/>
-      <c r="AE14" s="194"/>
-      <c r="AF14" s="194"/>
-      <c r="AG14" s="194"/>
-      <c r="AH14" s="194"/>
-      <c r="AI14" s="194"/>
-      <c r="AJ14" s="194"/>
-      <c r="AK14" s="194"/>
+      <c r="O14" s="195"/>
+      <c r="P14" s="195"/>
+      <c r="Q14" s="195"/>
+      <c r="R14" s="195"/>
+      <c r="S14" s="195"/>
+      <c r="T14" s="195"/>
+      <c r="U14" s="195"/>
+      <c r="V14" s="195"/>
+      <c r="W14" s="195"/>
+      <c r="X14" s="195"/>
+      <c r="Y14" s="195"/>
+      <c r="Z14" s="195"/>
+      <c r="AA14" s="195"/>
+      <c r="AB14" s="195"/>
+      <c r="AC14" s="195"/>
+      <c r="AD14" s="195"/>
+      <c r="AE14" s="195"/>
+      <c r="AF14" s="195"/>
+      <c r="AG14" s="195"/>
+      <c r="AH14" s="195"/>
+      <c r="AI14" s="195"/>
+      <c r="AJ14" s="195"/>
+      <c r="AK14" s="195"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -6052,43 +6137,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="195" t="s">
+      <c r="K15" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="L15" s="195"/>
-      <c r="M15" s="195"/>
-      <c r="N15" s="195"/>
-      <c r="O15" s="195"/>
-      <c r="P15" s="195"/>
-      <c r="Q15" s="195"/>
-      <c r="R15" s="195"/>
-      <c r="S15" s="195"/>
-      <c r="T15" s="195"/>
-      <c r="U15" s="195"/>
-      <c r="V15" s="195"/>
-      <c r="W15" s="195"/>
-      <c r="X15" s="195"/>
-      <c r="Y15" s="195"/>
-      <c r="Z15" s="195"/>
-      <c r="AA15" s="195"/>
-      <c r="AB15" s="195"/>
-      <c r="AC15" s="195"/>
-      <c r="AD15" s="195"/>
-      <c r="AE15" s="195"/>
-      <c r="AF15" s="195"/>
-      <c r="AG15" s="195"/>
-      <c r="AH15" s="195"/>
-      <c r="AI15" s="195"/>
-      <c r="AJ15" s="195"/>
-      <c r="AK15" s="195"/>
-      <c r="AL15" s="195"/>
-      <c r="AM15" s="195"/>
-      <c r="AN15" s="195"/>
-      <c r="AO15" s="195"/>
-      <c r="AP15" s="195"/>
-      <c r="AQ15" s="195"/>
-      <c r="AR15" s="195"/>
-      <c r="AS15" s="195"/>
+      <c r="L15" s="196"/>
+      <c r="M15" s="196"/>
+      <c r="N15" s="196"/>
+      <c r="O15" s="196"/>
+      <c r="P15" s="196"/>
+      <c r="Q15" s="196"/>
+      <c r="R15" s="196"/>
+      <c r="S15" s="196"/>
+      <c r="T15" s="196"/>
+      <c r="U15" s="196"/>
+      <c r="V15" s="196"/>
+      <c r="W15" s="196"/>
+      <c r="X15" s="196"/>
+      <c r="Y15" s="196"/>
+      <c r="Z15" s="196"/>
+      <c r="AA15" s="196"/>
+      <c r="AB15" s="196"/>
+      <c r="AC15" s="196"/>
+      <c r="AD15" s="196"/>
+      <c r="AE15" s="196"/>
+      <c r="AF15" s="196"/>
+      <c r="AG15" s="196"/>
+      <c r="AH15" s="196"/>
+      <c r="AI15" s="196"/>
+      <c r="AJ15" s="196"/>
+      <c r="AK15" s="196"/>
+      <c r="AL15" s="196"/>
+      <c r="AM15" s="196"/>
+      <c r="AN15" s="196"/>
+      <c r="AO15" s="196"/>
+      <c r="AP15" s="196"/>
+      <c r="AQ15" s="196"/>
+      <c r="AR15" s="196"/>
+      <c r="AS15" s="196"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -6108,41 +6193,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="195"/>
-      <c r="L16" s="195"/>
-      <c r="M16" s="195"/>
-      <c r="N16" s="195"/>
-      <c r="O16" s="195"/>
-      <c r="P16" s="195"/>
-      <c r="Q16" s="195"/>
-      <c r="R16" s="195"/>
-      <c r="S16" s="195"/>
-      <c r="T16" s="195"/>
-      <c r="U16" s="195"/>
-      <c r="V16" s="195"/>
-      <c r="W16" s="195"/>
-      <c r="X16" s="195"/>
-      <c r="Y16" s="195"/>
-      <c r="Z16" s="195"/>
-      <c r="AA16" s="195"/>
-      <c r="AB16" s="195"/>
-      <c r="AC16" s="195"/>
-      <c r="AD16" s="195"/>
-      <c r="AE16" s="195"/>
-      <c r="AF16" s="195"/>
-      <c r="AG16" s="195"/>
-      <c r="AH16" s="195"/>
-      <c r="AI16" s="195"/>
-      <c r="AJ16" s="195"/>
-      <c r="AK16" s="195"/>
-      <c r="AL16" s="195"/>
-      <c r="AM16" s="195"/>
-      <c r="AN16" s="195"/>
-      <c r="AO16" s="195"/>
-      <c r="AP16" s="195"/>
-      <c r="AQ16" s="195"/>
-      <c r="AR16" s="195"/>
-      <c r="AS16" s="195"/>
+      <c r="K16" s="196"/>
+      <c r="L16" s="196"/>
+      <c r="M16" s="196"/>
+      <c r="N16" s="196"/>
+      <c r="O16" s="196"/>
+      <c r="P16" s="196"/>
+      <c r="Q16" s="196"/>
+      <c r="R16" s="196"/>
+      <c r="S16" s="196"/>
+      <c r="T16" s="196"/>
+      <c r="U16" s="196"/>
+      <c r="V16" s="196"/>
+      <c r="W16" s="196"/>
+      <c r="X16" s="196"/>
+      <c r="Y16" s="196"/>
+      <c r="Z16" s="196"/>
+      <c r="AA16" s="196"/>
+      <c r="AB16" s="196"/>
+      <c r="AC16" s="196"/>
+      <c r="AD16" s="196"/>
+      <c r="AE16" s="196"/>
+      <c r="AF16" s="196"/>
+      <c r="AG16" s="196"/>
+      <c r="AH16" s="196"/>
+      <c r="AI16" s="196"/>
+      <c r="AJ16" s="196"/>
+      <c r="AK16" s="196"/>
+      <c r="AL16" s="196"/>
+      <c r="AM16" s="196"/>
+      <c r="AN16" s="196"/>
+      <c r="AO16" s="196"/>
+      <c r="AP16" s="196"/>
+      <c r="AQ16" s="196"/>
+      <c r="AR16" s="196"/>
+      <c r="AS16" s="196"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6731,14 +6816,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="196" t="s">
+      <c r="AN27" s="197" t="s">
         <v>125</v>
       </c>
-      <c r="AO27" s="196"/>
-      <c r="AP27" s="196"/>
-      <c r="AQ27" s="196"/>
-      <c r="AR27" s="196"/>
-      <c r="AS27" s="196"/>
+      <c r="AO27" s="197"/>
+      <c r="AP27" s="197"/>
+      <c r="AQ27" s="197"/>
+      <c r="AR27" s="197"/>
+      <c r="AS27" s="197"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7201,7 +7286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
@@ -7234,103 +7319,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="221" t="s">
+      <c r="F3" s="222" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -7369,7 +7454,7 @@
         <v>181</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L13" s="128"/>
       <c r="M13" s="128" t="s">
@@ -7391,23 +7476,23 @@
       <c r="S13" s="128"/>
     </row>
     <row r="14" spans="1:19" ht="14">
-      <c r="A14" s="188">
+      <c r="A14" s="184">
         <v>1</v>
       </c>
-      <c r="B14" s="189" t="s">
+      <c r="B14" s="185" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="190" t="s">
+      <c r="C14" s="186" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="190" t="s">
+      <c r="D14" s="186" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="191" t="s">
+      <c r="E14" s="187" t="s">
         <v>141</v>
       </c>
-      <c r="F14" s="192"/>
-      <c r="G14" s="193" t="s">
+      <c r="F14" s="188"/>
+      <c r="G14" s="189" t="s">
         <v>195</v>
       </c>
       <c r="H14" s="87"/>
@@ -7439,10 +7524,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>151</v>
@@ -7472,7 +7557,7 @@
         <v>135</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -7480,7 +7565,7 @@
       <c r="F16" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="187" t="s">
+      <c r="G16" s="183" t="s">
         <v>98</v>
       </c>
       <c r="H16" s="87"/>
@@ -7491,7 +7576,7 @@
         <v>111</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M16" s="13" t="s">
         <v>151</v>
@@ -7521,7 +7606,7 @@
         <v>183</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>141</v>
@@ -7558,48 +7643,48 @@
     </row>
     <row r="19" spans="1:18" ht="12" thickBot="1">
       <c r="A19" s="70"/>
-      <c r="B19" s="144"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="68"/>
-      <c r="D19" s="145"/>
+      <c r="D19" s="142"/>
       <c r="E19" s="131"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="147"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="144"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="148"/>
-      <c r="B20" s="149"/>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="152"/>
-      <c r="G20" s="153"/>
+      <c r="A20" s="145"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="147"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="149"/>
+      <c r="G20" s="150"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="148"/>
-      <c r="B21" s="149"/>
-      <c r="C21" s="154"/>
-      <c r="D21" s="150"/>
-      <c r="E21" s="151"/>
-      <c r="F21" s="152"/>
-      <c r="G21" s="153"/>
+      <c r="A21" s="145"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="151"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="149"/>
+      <c r="G21" s="150"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="148"/>
-      <c r="B22" s="149"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="153"/>
+      <c r="A22" s="145"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="148"/>
+      <c r="F22" s="149"/>
+      <c r="G22" s="150"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="148"/>
-      <c r="B23" s="155"/>
-      <c r="C23" s="156"/>
-      <c r="D23" s="156"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="159"/>
+      <c r="A23" s="145"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="153"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="155"/>
+      <c r="G23" s="156"/>
     </row>
     <row r="25" spans="1:18" ht="12" thickBot="1">
       <c r="A25" s="1" t="s">
@@ -7613,10 +7698,10 @@
       <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="205" t="s">
+      <c r="C26" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="206"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="34" t="s">
         <v>33</v>
       </c>
@@ -7628,66 +7713,66 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="13">
-      <c r="A27" s="160">
+      <c r="A27" s="157">
         <v>1</v>
       </c>
-      <c r="B27" s="161" t="s">
+      <c r="B27" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="236" t="s">
+      <c r="C27" s="237" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="237"/>
-      <c r="E27" s="162" t="s">
+      <c r="D27" s="238"/>
+      <c r="E27" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="162" t="s">
+      <c r="F27" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="163"/>
+      <c r="G27" s="160"/>
     </row>
     <row r="28" spans="1:18" ht="13">
-      <c r="A28" s="252"/>
+      <c r="A28" s="190"/>
       <c r="B28" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="253" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="191" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="254"/>
-      <c r="E28" s="255" t="s">
+      <c r="D28" s="192"/>
+      <c r="E28" s="193" t="s">
         <v>141</v>
       </c>
-      <c r="F28" s="255" t="s">
+      <c r="F28" s="193" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="256"/>
+      <c r="G28" s="194"/>
     </row>
     <row r="29" spans="1:18" ht="12" thickBot="1">
-      <c r="A29" s="164">
+      <c r="A29" s="161">
         <v>2</v>
       </c>
       <c r="B29" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="238" t="s">
+      <c r="C29" s="250" t="s">
         <v>173</v>
       </c>
-      <c r="D29" s="238"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="166"/>
-      <c r="G29" s="167" t="s">
+      <c r="D29" s="250"/>
+      <c r="E29" s="162"/>
+      <c r="F29" s="162"/>
+      <c r="G29" s="163" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="12" thickBot="1">
-      <c r="A30" s="168"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="250"/>
-      <c r="D30" s="251"/>
-      <c r="E30" s="170"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="171"/>
+      <c r="A30" s="164"/>
+      <c r="B30" s="165"/>
+      <c r="C30" s="251"/>
+      <c r="D30" s="252"/>
+      <c r="E30" s="166"/>
+      <c r="F30" s="166"/>
+      <c r="G30" s="167"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="1" t="s">
@@ -7704,34 +7789,34 @@
       <c r="B34" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="198" t="s">
+      <c r="C34" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="199"/>
-      <c r="E34" s="198" t="s">
+      <c r="D34" s="200"/>
+      <c r="E34" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="200"/>
+      <c r="F34" s="201"/>
       <c r="G34" s="38" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1">
-      <c r="A35" s="172">
+      <c r="A35" s="168">
         <v>1</v>
       </c>
-      <c r="B35" s="173" t="s">
+      <c r="B35" s="169" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="173" t="s">
+      <c r="C35" s="169" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="173"/>
-      <c r="E35" s="234" t="s">
+      <c r="D35" s="169"/>
+      <c r="E35" s="235" t="s">
         <v>176</v>
       </c>
-      <c r="F35" s="235"/>
-      <c r="G35" s="174" t="s">
+      <c r="F35" s="236"/>
+      <c r="G35" s="170" t="s">
         <v>113</v>
       </c>
     </row>
@@ -7747,14 +7832,14 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="198" t="s">
+      <c r="C38" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="199"/>
-      <c r="E38" s="198" t="s">
+      <c r="D38" s="200"/>
+      <c r="E38" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="200"/>
+      <c r="F38" s="201"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
@@ -8093,11 +8178,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
     </row>
     <row r="2" spans="1:3" ht="12" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -8360,10 +8445,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -8394,103 +8479,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="221" t="s">
+      <c r="F3" s="222" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8542,7 +8627,7 @@
         <v>122</v>
       </c>
       <c r="P13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q13" s="128" t="s">
         <v>135</v>
@@ -8592,7 +8677,7 @@
         <v>122</v>
       </c>
       <c r="P14" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q14" s="127">
         <v>41922.465277777781</v>
@@ -8642,7 +8727,7 @@
         <v>122</v>
       </c>
       <c r="P15" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q15" s="127">
         <v>41922.46875</v>
@@ -8730,7 +8815,7 @@
         <v>132</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -8751,67 +8836,67 @@
         <v>197</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="E20" s="66"/>
       <c r="F20" s="67"/>
       <c r="G20" s="133"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="59">
+      <c r="A21" s="253">
         <v>8</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="254" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="136" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="E21" s="66" t="s">
+      <c r="D21" s="136" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="255" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="67" t="s">
+      <c r="F21" s="256" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="106" t="s">
+      <c r="G21" s="139" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="59">
+    <row r="22" spans="1:7" s="257" customFormat="1" ht="12" thickBot="1">
+      <c r="A22" s="265">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="266" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="258" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="E22" s="66" t="s">
+      <c r="D22" s="258" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="259" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="67" t="s">
+      <c r="F22" s="260" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="106" t="s">
+      <c r="G22" s="261" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="148"/>
-      <c r="B23" s="149"/>
-      <c r="C23" s="150"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="153"/>
+      <c r="A23" s="145"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="149"/>
+      <c r="G23" s="150"/>
     </row>
     <row r="25" spans="1:7" ht="12" thickBot="1">
       <c r="A25" s="1" t="s">
@@ -8825,10 +8910,10 @@
       <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="205" t="s">
+      <c r="C26" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="206"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="34" t="s">
         <v>33</v>
       </c>
@@ -8846,10 +8931,10 @@
       <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="217" t="s">
+      <c r="C27" s="218" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="218"/>
+      <c r="D27" s="219"/>
       <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
@@ -8863,12 +8948,12 @@
         <v>2</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="C28" s="203" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="204" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="204"/>
+      <c r="D28" s="205"/>
       <c r="E28" s="52"/>
       <c r="F28" s="52" t="s">
         <v>141</v>
@@ -8877,102 +8962,68 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13" customHeight="1">
-      <c r="A29" s="57">
+    <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A29" s="56">
         <v>3</v>
       </c>
-      <c r="B29" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="134" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="135"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="136" customFormat="1" ht="13" customHeight="1">
-      <c r="A30" s="57">
-        <v>4</v>
-      </c>
-      <c r="B30" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="134" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30" s="135"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="53" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="13" customHeight="1" thickBot="1">
-      <c r="A31" s="56">
-        <v>5</v>
-      </c>
-      <c r="B31" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="C31" s="201" t="s">
+      <c r="B29" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="202" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="202"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58" t="s">
+      <c r="D29" s="203"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="G31" s="55"/>
-    </row>
-    <row r="33" spans="1:7" ht="12" thickBot="1">
-      <c r="A33" s="1" t="s">
+      <c r="G29" s="55"/>
+    </row>
+    <row r="31" spans="1:7" ht="12" thickBot="1">
+      <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14" thickBot="1">
-      <c r="A34" s="36" t="s">
+    <row r="32" spans="1:7" ht="14" thickBot="1">
+      <c r="A32" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="198" t="s">
+      <c r="C32" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="199"/>
-      <c r="E34" s="198" t="s">
+      <c r="D32" s="200"/>
+      <c r="E32" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="200"/>
-      <c r="G34" s="38" t="s">
+      <c r="F32" s="201"/>
+      <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12" thickBot="1">
-      <c r="A36" s="1" t="s">
+    <row r="34" spans="1:7" ht="12" thickBot="1">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="14" thickBot="1">
-      <c r="A37" s="36" t="s">
+    <row r="35" spans="1:7" ht="14" thickBot="1">
+      <c r="A35" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="198" t="s">
+      <c r="C35" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="199"/>
-      <c r="E37" s="198" t="s">
+      <c r="D35" s="200"/>
+      <c r="E35" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="200"/>
-      <c r="G37" s="38" t="s">
+      <c r="F35" s="201"/>
+      <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8989,15 +9040,15 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9045,103 +9096,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="223" t="s">
+      <c r="F3" s="224" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9363,10 +9414,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="205" t="s">
+      <c r="C24" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="206"/>
+      <c r="D24" s="207"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -9384,10 +9435,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="217" t="s">
+      <c r="C25" s="218" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="218"/>
+      <c r="D25" s="219"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -9401,10 +9452,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="228" t="s">
+      <c r="C26" s="229" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="229"/>
+      <c r="D26" s="230"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -9423,14 +9474,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="198" t="s">
+      <c r="C29" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="199"/>
-      <c r="E29" s="198" t="s">
+      <c r="D29" s="200"/>
+      <c r="E29" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="200"/>
+      <c r="F29" s="201"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -9447,14 +9498,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="198" t="s">
+      <c r="C32" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="199"/>
-      <c r="E32" s="198" t="s">
+      <c r="D32" s="200"/>
+      <c r="E32" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="200"/>
+      <c r="F32" s="201"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -9464,14 +9515,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="226" t="s">
+      <c r="C33" s="227" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="227"/>
-      <c r="E33" s="228" t="s">
+      <c r="D33" s="228"/>
+      <c r="E33" s="229" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="229"/>
+      <c r="F33" s="230"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
@@ -9546,105 +9597,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="223" t="s">
+      <c r="F3" s="224" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="210" t="s">
+      <c r="B8" s="211" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9749,10 +9800,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="205" t="s">
+      <c r="C19" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="206"/>
+      <c r="D19" s="207"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -9770,10 +9821,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="217" t="s">
+      <c r="C20" s="218" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="218"/>
+      <c r="D20" s="219"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -9787,10 +9838,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="226" t="s">
+      <c r="C21" s="227" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="227"/>
+      <c r="D21" s="228"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -9809,14 +9860,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="198" t="s">
+      <c r="C24" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="199"/>
-      <c r="E24" s="198" t="s">
+      <c r="D24" s="200"/>
+      <c r="E24" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="200"/>
+      <c r="F24" s="201"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -9833,14 +9884,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="198" t="s">
+      <c r="C27" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="199"/>
-      <c r="E27" s="198" t="s">
+      <c r="D27" s="200"/>
+      <c r="E27" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="200"/>
+      <c r="F27" s="201"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -9850,10 +9901,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="226"/>
-      <c r="D28" s="227"/>
-      <c r="E28" s="228"/>
-      <c r="F28" s="229"/>
+      <c r="C28" s="227"/>
+      <c r="D28" s="228"/>
+      <c r="E28" s="229"/>
+      <c r="F28" s="230"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
@@ -9926,103 +9977,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="232" t="s">
+      <c r="F2" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="233"/>
+      <c r="G2" s="234"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="221" t="s">
+      <c r="F3" s="222" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -10238,10 +10289,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="205" t="s">
+      <c r="C21" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="206"/>
+      <c r="D21" s="207"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -10265,10 +10316,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="217" t="s">
+      <c r="C22" s="218" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="218"/>
+      <c r="D22" s="219"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -10288,10 +10339,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="203" t="s">
+      <c r="C23" s="204" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="204"/>
+      <c r="D23" s="205"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -10309,10 +10360,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="226" t="s">
+      <c r="C24" s="227" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="227"/>
+      <c r="D24" s="228"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -10351,14 +10402,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="198" t="s">
+      <c r="C27" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="199"/>
-      <c r="E27" s="198" t="s">
+      <c r="D27" s="200"/>
+      <c r="E27" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="200"/>
+      <c r="F27" s="201"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -10395,14 +10446,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="198" t="s">
+      <c r="C30" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="199"/>
-      <c r="E30" s="198" t="s">
+      <c r="D30" s="200"/>
+      <c r="E30" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="200"/>
+      <c r="F30" s="201"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -10418,14 +10469,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="217" t="s">
+      <c r="C31" s="218" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="218"/>
-      <c r="E31" s="203" t="s">
+      <c r="D31" s="219"/>
+      <c r="E31" s="204" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="204"/>
+      <c r="F31" s="205"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -10441,14 +10492,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="230" t="s">
+      <c r="C32" s="231" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="231"/>
-      <c r="E32" s="228" t="s">
+      <c r="D32" s="232"/>
+      <c r="E32" s="229" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="229"/>
+      <c r="F32" s="230"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -10543,10 +10594,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -10577,103 +10628,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="221" t="s">
+      <c r="F3" s="222" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10718,7 +10769,7 @@
         <v>155</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N13" s="128" t="s">
         <v>149</v>
@@ -10727,7 +10778,7 @@
         <v>149</v>
       </c>
       <c r="P13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q13" s="128" t="s">
         <v>135</v>
@@ -10764,13 +10815,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M14" s="13" t="s">
         <v>151</v>
@@ -10782,7 +10833,7 @@
         <v>149</v>
       </c>
       <c r="P14" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q14" s="127">
         <v>41922.465277777781</v>
@@ -10818,13 +10869,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>151</v>
@@ -10836,7 +10887,7 @@
         <v>149</v>
       </c>
       <c r="P15" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q15" s="127">
         <v>41922.46875</v>
@@ -10904,7 +10955,7 @@
         <v>157</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
@@ -10921,22 +10972,22 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="137" t="s">
+      <c r="B19" s="134" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="135" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="139" t="s">
-        <v>199</v>
-      </c>
-      <c r="E19" s="140" t="s">
+      <c r="D19" s="136" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="141" t="s">
+      <c r="F19" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="142" t="s">
+      <c r="G19" s="139" t="s">
         <v>159</v>
       </c>
     </row>
@@ -10953,7 +11004,7 @@
       <c r="D20" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="143" t="s">
+      <c r="E20" s="140" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="22"/>
@@ -10965,67 +11016,67 @@
       <c r="A21" s="59">
         <v>7</v>
       </c>
-      <c r="B21" s="137" t="s">
+      <c r="B21" s="134" t="s">
         <v>196</v>
       </c>
-      <c r="C21" s="138" t="s">
+      <c r="C21" s="135" t="s">
         <v>197</v>
       </c>
-      <c r="D21" s="139" t="s">
-        <v>198</v>
-      </c>
-      <c r="E21" s="140"/>
-      <c r="F21" s="141"/>
-      <c r="G21" s="142"/>
+      <c r="D21" s="136" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="137"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="139"/>
     </row>
     <row r="22" spans="1:8" ht="12" thickBot="1">
       <c r="A22" s="70">
         <f>A20+1</f>
         <v>9</v>
       </c>
-      <c r="B22" s="144" t="s">
+      <c r="B22" s="141" t="s">
         <v>172</v>
       </c>
       <c r="C22" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="D22" s="145" t="s">
+      <c r="D22" s="142" t="s">
         <v>161</v>
       </c>
       <c r="E22" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="146"/>
-      <c r="G22" s="147" t="s">
+      <c r="F22" s="143"/>
+      <c r="G22" s="144" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="148"/>
-      <c r="B23" s="149"/>
-      <c r="C23" s="150"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="153"/>
+      <c r="A23" s="145"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="148"/>
+      <c r="F23" s="149"/>
+      <c r="G23" s="150"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="148"/>
-      <c r="B25" s="149"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="152"/>
-      <c r="G25" s="153"/>
+      <c r="A25" s="145"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="147"/>
+      <c r="D25" s="147"/>
+      <c r="E25" s="148"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="150"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="148"/>
-      <c r="B26" s="155"/>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="157"/>
-      <c r="F26" s="158"/>
-      <c r="G26" s="159"/>
+      <c r="A26" s="145"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="153"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="156"/>
     </row>
     <row r="28" spans="1:8" ht="12" thickBot="1">
       <c r="A28" s="1" t="s">
@@ -11039,10 +11090,10 @@
       <c r="B29" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="205" t="s">
+      <c r="C29" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="206"/>
+      <c r="D29" s="207"/>
       <c r="E29" s="34" t="s">
         <v>33</v>
       </c>
@@ -11054,130 +11105,113 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="13">
-      <c r="A30" s="160">
+      <c r="A30" s="157">
         <v>1</v>
       </c>
-      <c r="B30" s="161" t="s">
+      <c r="B30" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="236" t="s">
+      <c r="C30" s="237" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="237"/>
-      <c r="E30" s="162" t="s">
+      <c r="D30" s="238"/>
+      <c r="E30" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="162" t="s">
+      <c r="F30" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="163"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="G30" s="160"/>
+    </row>
+    <row r="31" spans="1:8" ht="12" thickBot="1">
       <c r="A31" s="164">
         <v>2</v>
       </c>
       <c r="B31" s="165" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="238" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="238"/>
+        <v>194</v>
+      </c>
+      <c r="C31" s="239" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="239"/>
       <c r="E31" s="166"/>
       <c r="F31" s="166"/>
       <c r="G31" s="167" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12" thickBot="1">
-      <c r="A32" s="168">
-        <v>3</v>
-      </c>
-      <c r="B32" s="169" t="s">
-        <v>194</v>
-      </c>
-      <c r="C32" s="239" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="12" thickBot="1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" ht="14" thickBot="1">
+      <c r="A35" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="199" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="200"/>
+      <c r="E35" s="199" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="201"/>
+      <c r="G35" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1">
+      <c r="A36" s="168">
+        <v>1</v>
+      </c>
+      <c r="B36" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="169" t="s">
         <v>173</v>
       </c>
-      <c r="D32" s="239"/>
-      <c r="E32" s="170"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="171" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="12" thickBot="1">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" ht="14" thickBot="1">
-      <c r="A36" s="36" t="s">
+      <c r="D36" s="169"/>
+      <c r="E36" s="235" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="236"/>
+      <c r="G36" s="170" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="12" thickBot="1">
+      <c r="A38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="14" thickBot="1">
+      <c r="A39" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="198" t="s">
+      <c r="C39" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="199"/>
-      <c r="E36" s="198" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="200"/>
-      <c r="G36" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1">
-      <c r="A37" s="172">
-        <v>1</v>
-      </c>
-      <c r="B37" s="173" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" s="173" t="s">
-        <v>173</v>
-      </c>
-      <c r="D37" s="173"/>
-      <c r="E37" s="234" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="235"/>
-      <c r="G37" s="174" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="12" thickBot="1">
-      <c r="A39" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="14" thickBot="1">
-      <c r="A40" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="199"/>
-      <c r="E40" s="198" t="s">
+      <c r="D39" s="200"/>
+      <c r="E39" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F40" s="200"/>
-      <c r="G40" s="38" t="s">
+      <c r="F39" s="201"/>
+      <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11190,15 +11224,14 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11214,8 +11247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -11246,103 +11279,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="219" t="s">
+      <c r="C2" s="220" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="224"/>
+      <c r="D2" s="225"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="219" t="s">
+      <c r="F2" s="220" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="220"/>
+      <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="221" t="s">
+      <c r="F3" s="222" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="222"/>
+      <c r="G3" s="223"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="224" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="225"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="G4" s="222"/>
+      <c r="F4" s="224"/>
+      <c r="G4" s="223"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="224" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="225"/>
+      <c r="D5" s="226"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="223"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="224" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="225"/>
+      <c r="D6" s="226"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="222"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="223"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="208" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="208"/>
-      <c r="E7" s="208"/>
-      <c r="F7" s="208"/>
-      <c r="G7" s="209"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="210"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="210"/>
-      <c r="C8" s="211"/>
-      <c r="D8" s="211"/>
-      <c r="E8" s="211"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="212"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
+      <c r="G8" s="213"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="213"/>
-      <c r="C9" s="211"/>
-      <c r="D9" s="211"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="211"/>
-      <c r="G9" s="212"/>
+      <c r="B9" s="214"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="213"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="214"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="216"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="216"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11381,10 +11414,10 @@
         <v>155</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M13" s="128" t="s">
         <v>149</v>
@@ -11396,7 +11429,7 @@
         <v>149</v>
       </c>
       <c r="P13" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q13" s="128" t="s">
         <v>135</v>
@@ -11431,13 +11464,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M14" s="13" t="s">
         <v>151</v>
@@ -11449,7 +11482,7 @@
         <v>149</v>
       </c>
       <c r="P14" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q14" s="127">
         <v>41922.465277777781</v>
@@ -11484,13 +11517,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>151</v>
@@ -11502,7 +11535,7 @@
         <v>149</v>
       </c>
       <c r="P15" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q15" s="127">
         <v>41922.46875</v>
@@ -11523,7 +11556,7 @@
         <v>135</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -11531,12 +11564,12 @@
       <c r="F16" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="G16" s="139" t="s">
         <v>98</v>
       </c>
       <c r="H16" s="87"/>
     </row>
-    <row r="17" spans="1:7" ht="12" thickBot="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="59">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -11548,15 +11581,15 @@
         <v>136</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="262" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="186" t="s">
+      <c r="G17" s="264" t="s">
         <v>159</v>
       </c>
     </row>
@@ -11577,14 +11610,15 @@
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
+      <c r="G18" s="263"/>
     </row>
     <row r="19" spans="1:7" ht="12" thickBot="1">
       <c r="A19" s="70">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="144" t="s">
-        <v>200</v>
+      <c r="B19" s="141" t="s">
+        <v>199</v>
       </c>
       <c r="C19" s="68" t="s">
         <v>192</v>
@@ -11595,8 +11629,8 @@
       <c r="E19" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="175"/>
-      <c r="G19" s="186"/>
+      <c r="F19" s="171"/>
+      <c r="G19" s="182"/>
     </row>
     <row r="21" spans="1:7" ht="12" thickBot="1">
       <c r="A21" s="1" t="s">
@@ -11610,10 +11644,10 @@
       <c r="B22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="205" t="s">
+      <c r="C22" s="206" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="206"/>
+      <c r="D22" s="207"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -11625,23 +11659,23 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="13">
-      <c r="A23" s="176">
+      <c r="A23" s="172">
         <v>1</v>
       </c>
-      <c r="B23" s="177" t="s">
+      <c r="B23" s="173" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="246" t="s">
         <v>113</v>
       </c>
       <c r="D23" s="247"/>
-      <c r="E23" s="178" t="s">
+      <c r="E23" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="178" t="s">
+      <c r="F23" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="179"/>
+      <c r="G23" s="175"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="15">
@@ -11689,23 +11723,23 @@
       <c r="B28" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="198" t="s">
+      <c r="C28" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="199"/>
-      <c r="E28" s="198" t="s">
+      <c r="D28" s="200"/>
+      <c r="E28" s="199" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="200"/>
+      <c r="F28" s="201"/>
       <c r="G28" s="38" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="180">
+      <c r="A29" s="176">
         <v>1</v>
       </c>
-      <c r="B29" s="181" t="s">
+      <c r="B29" s="177" t="s">
         <v>188</v>
       </c>
       <c r="C29" s="240" t="s">
@@ -11716,15 +11750,15 @@
         <v>175</v>
       </c>
       <c r="F29" s="242"/>
-      <c r="G29" s="182" t="s">
+      <c r="G29" s="178" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12" thickBot="1">
-      <c r="A30" s="183">
+      <c r="A30" s="179">
         <v>2</v>
       </c>
-      <c r="B30" s="184" t="s">
+      <c r="B30" s="180" t="s">
         <v>189</v>
       </c>
       <c r="C30" s="243" t="s">
@@ -11735,7 +11769,7 @@
         <v>176</v>
       </c>
       <c r="F30" s="245"/>
-      <c r="G30" s="185" t="s">
+      <c r="G30" s="181" t="s">
         <v>113</v>
       </c>
     </row>
@@ -11751,14 +11785,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="198" t="s">
+      <c r="C33" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="199"/>
-      <c r="E33" s="198" t="s">
+      <c r="D33" s="200"/>
+      <c r="E33" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="200"/>
+      <c r="F33" s="201"/>
       <c r="G33" s="38" t="s">
         <v>39</v>
       </c>

</xml_diff>